<commit_message>
RORPractitioner.fsh test  \n 42fced5323a549d1922dc18cf2fe592e69bd4b0d
</commit_message>
<xml_diff>
--- a/sg/mappingFHIR-ROR/ig/StructureDefinition-ror-organization.xlsx
+++ b/sg/mappingFHIR-ROR/ig/StructureDefinition-ror-organization.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9652" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9653" uniqueCount="1022">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-24T16:23:30+00:00</t>
+    <t>2026-01-05T09:58:39+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2369,6 +2369,9 @@
   </si>
   <si>
     <t>Organization.address.extension:ror-organization-geolocation.extension</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and managable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
   </si>
   <si>
     <t>Organization.address.extension:ror-organization-geolocation.extension:latitude</t>
@@ -24665,7 +24668,7 @@
       </c>
       <c r="C190" s="2"/>
       <c r="D190" t="s" s="2">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="E190" s="2"/>
       <c r="F190" t="s" s="2">
@@ -24687,12 +24690,14 @@
         <v>109</v>
       </c>
       <c r="L190" t="s" s="2">
-        <v>194</v>
+        <v>110</v>
       </c>
       <c r="M190" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="N190" s="2"/>
+        <v>748</v>
+      </c>
+      <c r="N190" t="s" s="2">
+        <v>112</v>
+      </c>
       <c r="O190" s="2"/>
       <c r="P190" t="s" s="2">
         <v>75</v>
@@ -24767,13 +24772,13 @@
     </row>
     <row r="191" hidden="true">
       <c r="A191" t="s" s="2">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B191" t="s" s="2">
         <v>732</v>
       </c>
       <c r="C191" t="s" s="2">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="D191" t="s" s="2">
         <v>75</v>
@@ -24798,10 +24803,10 @@
         <v>109</v>
       </c>
       <c r="L191" t="s" s="2">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="M191" t="s" s="2">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="N191" s="2"/>
       <c r="O191" s="2"/>
@@ -24878,10 +24883,10 @@
     </row>
     <row r="192" hidden="true">
       <c r="A192" t="s" s="2">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B192" t="s" s="2">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="C192" s="2"/>
       <c r="D192" t="s" s="2">
@@ -24987,10 +24992,10 @@
     </row>
     <row r="193" hidden="true">
       <c r="A193" t="s" s="2">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B193" t="s" s="2">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C193" s="2"/>
       <c r="D193" t="s" s="2">
@@ -25096,10 +25101,10 @@
     </row>
     <row r="194" hidden="true">
       <c r="A194" t="s" s="2">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B194" t="s" s="2">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C194" s="2"/>
       <c r="D194" t="s" s="2">
@@ -25139,7 +25144,7 @@
       </c>
       <c r="Q194" s="2"/>
       <c r="R194" t="s" s="2">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="S194" t="s" s="2">
         <v>75</v>
@@ -25207,10 +25212,10 @@
     </row>
     <row r="195" hidden="true">
       <c r="A195" t="s" s="2">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B195" t="s" s="2">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C195" s="2"/>
       <c r="D195" t="s" s="2">
@@ -25233,7 +25238,7 @@
         <v>75</v>
       </c>
       <c r="K195" t="s" s="2">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="L195" t="s" s="2">
         <v>225</v>
@@ -25316,13 +25321,13 @@
     </row>
     <row r="196" hidden="true">
       <c r="A196" t="s" s="2">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B196" t="s" s="2">
         <v>732</v>
       </c>
       <c r="C196" t="s" s="2">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="D196" t="s" s="2">
         <v>75</v>
@@ -25347,10 +25352,10 @@
         <v>109</v>
       </c>
       <c r="L196" t="s" s="2">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="M196" t="s" s="2">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="N196" s="2"/>
       <c r="O196" s="2"/>
@@ -25427,10 +25432,10 @@
     </row>
     <row r="197" hidden="true">
       <c r="A197" t="s" s="2">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B197" t="s" s="2">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="C197" s="2"/>
       <c r="D197" t="s" s="2">
@@ -25536,10 +25541,10 @@
     </row>
     <row r="198" hidden="true">
       <c r="A198" t="s" s="2">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B198" t="s" s="2">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C198" s="2"/>
       <c r="D198" t="s" s="2">
@@ -25645,10 +25650,10 @@
     </row>
     <row r="199" hidden="true">
       <c r="A199" t="s" s="2">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B199" t="s" s="2">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C199" s="2"/>
       <c r="D199" t="s" s="2">
@@ -25688,7 +25693,7 @@
       </c>
       <c r="Q199" s="2"/>
       <c r="R199" t="s" s="2">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="S199" t="s" s="2">
         <v>75</v>
@@ -25756,10 +25761,10 @@
     </row>
     <row r="200" hidden="true">
       <c r="A200" t="s" s="2">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B200" t="s" s="2">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C200" s="2"/>
       <c r="D200" t="s" s="2">
@@ -25782,7 +25787,7 @@
         <v>75</v>
       </c>
       <c r="K200" t="s" s="2">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="L200" t="s" s="2">
         <v>225</v>
@@ -25865,13 +25870,13 @@
     </row>
     <row r="201" hidden="true">
       <c r="A201" t="s" s="2">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B201" t="s" s="2">
         <v>732</v>
       </c>
       <c r="C201" t="s" s="2">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="D201" t="s" s="2">
         <v>75</v>
@@ -25893,13 +25898,13 @@
         <v>75</v>
       </c>
       <c r="K201" t="s" s="2">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="L201" t="s" s="2">
         <v>194</v>
       </c>
       <c r="M201" t="s" s="2">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="N201" s="2"/>
       <c r="O201" s="2"/>
@@ -25976,7 +25981,7 @@
     </row>
     <row r="202" hidden="true">
       <c r="A202" t="s" s="2">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B202" t="s" s="2">
         <v>734</v>
@@ -26019,7 +26024,7 @@
       </c>
       <c r="Q202" s="2"/>
       <c r="R202" t="s" s="2">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="S202" t="s" s="2">
         <v>75</v>
@@ -26087,7 +26092,7 @@
     </row>
     <row r="203" hidden="true">
       <c r="A203" t="s" s="2">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B203" t="s" s="2">
         <v>737</v>
@@ -26113,7 +26118,7 @@
         <v>75</v>
       </c>
       <c r="K203" t="s" s="2">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="L203" t="s" s="2">
         <v>225</v>
@@ -26196,10 +26201,10 @@
     </row>
     <row r="204" hidden="true">
       <c r="A204" t="s" s="2">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B204" t="s" s="2">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C204" s="2"/>
       <c r="D204" t="s" s="2">
@@ -26225,16 +26230,16 @@
         <v>171</v>
       </c>
       <c r="L204" t="s" s="2">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="M204" t="s" s="2">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="N204" t="s" s="2">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="O204" t="s" s="2">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="P204" t="s" s="2">
         <v>75</v>
@@ -26247,7 +26252,7 @@
         <v>75</v>
       </c>
       <c r="T204" t="s" s="2">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="U204" t="s" s="2">
         <v>75</v>
@@ -26262,10 +26267,10 @@
         <v>162</v>
       </c>
       <c r="Y204" t="s" s="2">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="Z204" t="s" s="2">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="AA204" t="s" s="2">
         <v>75</v>
@@ -26283,7 +26288,7 @@
         <v>75</v>
       </c>
       <c r="AF204" t="s" s="2">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="AG204" t="s" s="2">
         <v>76</v>
@@ -26309,10 +26314,10 @@
     </row>
     <row r="205" hidden="true">
       <c r="A205" t="s" s="2">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B205" t="s" s="2">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C205" s="2"/>
       <c r="D205" t="s" s="2">
@@ -26338,13 +26343,13 @@
         <v>171</v>
       </c>
       <c r="L205" t="s" s="2">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="M205" t="s" s="2">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="N205" t="s" s="2">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="O205" s="2"/>
       <c r="P205" t="s" s="2">
@@ -26358,7 +26363,7 @@
         <v>75</v>
       </c>
       <c r="T205" t="s" s="2">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="U205" t="s" s="2">
         <v>75</v>
@@ -26373,10 +26378,10 @@
         <v>162</v>
       </c>
       <c r="Y205" t="s" s="2">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="Z205" t="s" s="2">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="AA205" t="s" s="2">
         <v>75</v>
@@ -26394,7 +26399,7 @@
         <v>75</v>
       </c>
       <c r="AF205" t="s" s="2">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="AG205" t="s" s="2">
         <v>76</v>
@@ -26420,10 +26425,10 @@
     </row>
     <row r="206" hidden="true">
       <c r="A206" t="s" s="2">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B206" t="s" s="2">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C206" s="2"/>
       <c r="D206" t="s" s="2">
@@ -26449,16 +26454,16 @@
         <v>103</v>
       </c>
       <c r="L206" t="s" s="2">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="M206" t="s" s="2">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="N206" t="s" s="2">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="O206" t="s" s="2">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="P206" t="s" s="2">
         <v>75</v>
@@ -26471,7 +26476,7 @@
         <v>75</v>
       </c>
       <c r="T206" t="s" s="2">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="U206" t="s" s="2">
         <v>75</v>
@@ -26507,7 +26512,7 @@
         <v>75</v>
       </c>
       <c r="AF206" t="s" s="2">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="AG206" t="s" s="2">
         <v>76</v>
@@ -26533,10 +26538,10 @@
     </row>
     <row r="207" hidden="true">
       <c r="A207" t="s" s="2">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B207" t="s" s="2">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C207" s="2"/>
       <c r="D207" t="s" s="2">
@@ -26562,10 +26567,10 @@
         <v>103</v>
       </c>
       <c r="L207" t="s" s="2">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="M207" t="s" s="2">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="N207" t="s" s="2">
         <v>544</v>
@@ -26582,7 +26587,7 @@
         <v>75</v>
       </c>
       <c r="T207" t="s" s="2">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="U207" t="s" s="2">
         <v>75</v>
@@ -26618,7 +26623,7 @@
         <v>75</v>
       </c>
       <c r="AF207" t="s" s="2">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="AG207" t="s" s="2">
         <v>76</v>
@@ -26644,10 +26649,10 @@
     </row>
     <row r="208" hidden="true">
       <c r="A208" t="s" s="2">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="B208" t="s" s="2">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C208" s="2"/>
       <c r="D208" t="s" s="2">
@@ -26753,10 +26758,10 @@
     </row>
     <row r="209" hidden="true">
       <c r="A209" t="s" s="2">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B209" t="s" s="2">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C209" s="2"/>
       <c r="D209" t="s" s="2">
@@ -26864,13 +26869,13 @@
     </row>
     <row r="210" hidden="true">
       <c r="A210" t="s" s="2">
+        <v>809</v>
+      </c>
+      <c r="B210" t="s" s="2">
         <v>808</v>
       </c>
-      <c r="B210" t="s" s="2">
-        <v>807</v>
-      </c>
       <c r="C210" t="s" s="2">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="D210" t="s" s="2">
         <v>75</v>
@@ -26892,13 +26897,13 @@
         <v>75</v>
       </c>
       <c r="K210" t="s" s="2">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="L210" t="s" s="2">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="M210" t="s" s="2">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="N210" s="2"/>
       <c r="O210" s="2"/>
@@ -26964,7 +26969,7 @@
         <v>117</v>
       </c>
       <c r="AK210" t="s" s="2">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="AL210" t="s" s="2">
         <v>75</v>
@@ -26975,13 +26980,13 @@
     </row>
     <row r="211" hidden="true">
       <c r="A211" t="s" s="2">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="B211" t="s" s="2">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C211" t="s" s="2">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D211" t="s" s="2">
         <v>75</v>
@@ -27003,13 +27008,13 @@
         <v>75</v>
       </c>
       <c r="K211" t="s" s="2">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="L211" t="s" s="2">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="M211" t="s" s="2">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="N211" s="2"/>
       <c r="O211" s="2"/>
@@ -27075,7 +27080,7 @@
         <v>117</v>
       </c>
       <c r="AK211" t="s" s="2">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="AL211" t="s" s="2">
         <v>75</v>
@@ -27086,13 +27091,13 @@
     </row>
     <row r="212" hidden="true">
       <c r="A212" t="s" s="2">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="B212" t="s" s="2">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C212" t="s" s="2">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D212" t="s" s="2">
         <v>75</v>
@@ -27114,13 +27119,13 @@
         <v>75</v>
       </c>
       <c r="K212" t="s" s="2">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="L212" t="s" s="2">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="M212" t="s" s="2">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="N212" s="2"/>
       <c r="O212" s="2"/>
@@ -27186,7 +27191,7 @@
         <v>117</v>
       </c>
       <c r="AK212" t="s" s="2">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="AL212" t="s" s="2">
         <v>75</v>
@@ -27197,13 +27202,13 @@
     </row>
     <row r="213" hidden="true">
       <c r="A213" t="s" s="2">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B213" t="s" s="2">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C213" t="s" s="2">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="D213" t="s" s="2">
         <v>75</v>
@@ -27225,13 +27230,13 @@
         <v>75</v>
       </c>
       <c r="K213" t="s" s="2">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="L213" t="s" s="2">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="M213" t="s" s="2">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="N213" s="2"/>
       <c r="O213" s="2"/>
@@ -27308,10 +27313,10 @@
     </row>
     <row r="214" hidden="true">
       <c r="A214" t="s" s="2">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="B214" t="s" s="2">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C214" s="2"/>
       <c r="D214" t="s" s="2">
@@ -27417,10 +27422,10 @@
     </row>
     <row r="215" hidden="true">
       <c r="A215" t="s" s="2">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B215" t="s" s="2">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C215" s="2"/>
       <c r="D215" t="s" s="2">
@@ -27526,10 +27531,10 @@
     </row>
     <row r="216" hidden="true">
       <c r="A216" t="s" s="2">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="B216" t="s" s="2">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C216" s="2"/>
       <c r="D216" t="s" s="2">
@@ -27569,7 +27574,7 @@
       </c>
       <c r="Q216" s="2"/>
       <c r="R216" t="s" s="2">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="S216" t="s" s="2">
         <v>75</v>
@@ -27637,10 +27642,10 @@
     </row>
     <row r="217" hidden="true">
       <c r="A217" t="s" s="2">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B217" t="s" s="2">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C217" s="2"/>
       <c r="D217" t="s" s="2">
@@ -27735,7 +27740,7 @@
         <v>100</v>
       </c>
       <c r="AK217" t="s" s="2">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="AL217" t="s" s="2">
         <v>75</v>
@@ -27746,13 +27751,13 @@
     </row>
     <row r="218" hidden="true">
       <c r="A218" t="s" s="2">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B218" t="s" s="2">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C218" t="s" s="2">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="D218" t="s" s="2">
         <v>75</v>
@@ -27774,13 +27779,13 @@
         <v>75</v>
       </c>
       <c r="K218" t="s" s="2">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="L218" t="s" s="2">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="M218" t="s" s="2">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="N218" s="2"/>
       <c r="O218" s="2"/>
@@ -27857,10 +27862,10 @@
     </row>
     <row r="219" hidden="true">
       <c r="A219" t="s" s="2">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B219" t="s" s="2">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C219" s="2"/>
       <c r="D219" t="s" s="2">
@@ -27966,10 +27971,10 @@
     </row>
     <row r="220" hidden="true">
       <c r="A220" t="s" s="2">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B220" t="s" s="2">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C220" s="2"/>
       <c r="D220" t="s" s="2">
@@ -28075,10 +28080,10 @@
     </row>
     <row r="221" hidden="true">
       <c r="A221" t="s" s="2">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B221" t="s" s="2">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C221" s="2"/>
       <c r="D221" t="s" s="2">
@@ -28118,7 +28123,7 @@
       </c>
       <c r="Q221" s="2"/>
       <c r="R221" t="s" s="2">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="S221" t="s" s="2">
         <v>75</v>
@@ -28186,10 +28191,10 @@
     </row>
     <row r="222" hidden="true">
       <c r="A222" t="s" s="2">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B222" t="s" s="2">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C222" s="2"/>
       <c r="D222" t="s" s="2">
@@ -28249,7 +28254,7 @@
       </c>
       <c r="Y222" s="2"/>
       <c r="Z222" t="s" s="2">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="AA222" t="s" s="2">
         <v>75</v>
@@ -28282,7 +28287,7 @@
         <v>100</v>
       </c>
       <c r="AK222" t="s" s="2">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="AL222" t="s" s="2">
         <v>75</v>
@@ -28293,13 +28298,13 @@
     </row>
     <row r="223" hidden="true">
       <c r="A223" t="s" s="2">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="B223" t="s" s="2">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C223" t="s" s="2">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="D223" t="s" s="2">
         <v>75</v>
@@ -28321,13 +28326,13 @@
         <v>75</v>
       </c>
       <c r="K223" t="s" s="2">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="L223" t="s" s="2">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="M223" t="s" s="2">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="N223" s="2"/>
       <c r="O223" s="2"/>
@@ -28404,10 +28409,10 @@
     </row>
     <row r="224" hidden="true">
       <c r="A224" t="s" s="2">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B224" t="s" s="2">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C224" s="2"/>
       <c r="D224" t="s" s="2">
@@ -28513,10 +28518,10 @@
     </row>
     <row r="225" hidden="true">
       <c r="A225" t="s" s="2">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B225" t="s" s="2">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C225" s="2"/>
       <c r="D225" t="s" s="2">
@@ -28622,10 +28627,10 @@
     </row>
     <row r="226" hidden="true">
       <c r="A226" t="s" s="2">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B226" t="s" s="2">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C226" s="2"/>
       <c r="D226" t="s" s="2">
@@ -28665,7 +28670,7 @@
       </c>
       <c r="Q226" s="2"/>
       <c r="R226" t="s" s="2">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="S226" t="s" s="2">
         <v>75</v>
@@ -28733,10 +28738,10 @@
     </row>
     <row r="227" hidden="true">
       <c r="A227" t="s" s="2">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B227" t="s" s="2">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C227" s="2"/>
       <c r="D227" t="s" s="2">
@@ -28831,7 +28836,7 @@
         <v>100</v>
       </c>
       <c r="AK227" t="s" s="2">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="AL227" t="s" s="2">
         <v>75</v>
@@ -28842,13 +28847,13 @@
     </row>
     <row r="228" hidden="true">
       <c r="A228" t="s" s="2">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B228" t="s" s="2">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C228" t="s" s="2">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="D228" t="s" s="2">
         <v>75</v>
@@ -28870,13 +28875,13 @@
         <v>75</v>
       </c>
       <c r="K228" t="s" s="2">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="L228" t="s" s="2">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="M228" t="s" s="2">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="N228" s="2"/>
       <c r="O228" s="2"/>
@@ -28953,10 +28958,10 @@
     </row>
     <row r="229" hidden="true">
       <c r="A229" t="s" s="2">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="B229" t="s" s="2">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C229" s="2"/>
       <c r="D229" t="s" s="2">
@@ -29062,10 +29067,10 @@
     </row>
     <row r="230" hidden="true">
       <c r="A230" t="s" s="2">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B230" t="s" s="2">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C230" s="2"/>
       <c r="D230" t="s" s="2">
@@ -29171,10 +29176,10 @@
     </row>
     <row r="231" hidden="true">
       <c r="A231" t="s" s="2">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B231" t="s" s="2">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C231" s="2"/>
       <c r="D231" t="s" s="2">
@@ -29214,7 +29219,7 @@
       </c>
       <c r="Q231" s="2"/>
       <c r="R231" t="s" s="2">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="S231" t="s" s="2">
         <v>75</v>
@@ -29282,10 +29287,10 @@
     </row>
     <row r="232" hidden="true">
       <c r="A232" t="s" s="2">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="B232" t="s" s="2">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C232" s="2"/>
       <c r="D232" t="s" s="2">
@@ -29380,7 +29385,7 @@
         <v>100</v>
       </c>
       <c r="AK232" t="s" s="2">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="AL232" t="s" s="2">
         <v>75</v>
@@ -29391,13 +29396,13 @@
     </row>
     <row r="233" hidden="true">
       <c r="A233" t="s" s="2">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="B233" t="s" s="2">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C233" t="s" s="2">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="D233" t="s" s="2">
         <v>75</v>
@@ -29419,13 +29424,13 @@
         <v>75</v>
       </c>
       <c r="K233" t="s" s="2">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="L233" t="s" s="2">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="M233" t="s" s="2">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="N233" s="2"/>
       <c r="O233" s="2"/>
@@ -29502,10 +29507,10 @@
     </row>
     <row r="234" hidden="true">
       <c r="A234" t="s" s="2">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="B234" t="s" s="2">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C234" s="2"/>
       <c r="D234" t="s" s="2">
@@ -29611,10 +29616,10 @@
     </row>
     <row r="235" hidden="true">
       <c r="A235" t="s" s="2">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B235" t="s" s="2">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C235" s="2"/>
       <c r="D235" t="s" s="2">
@@ -29720,10 +29725,10 @@
     </row>
     <row r="236" hidden="true">
       <c r="A236" t="s" s="2">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B236" t="s" s="2">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C236" s="2"/>
       <c r="D236" t="s" s="2">
@@ -29763,7 +29768,7 @@
       </c>
       <c r="Q236" s="2"/>
       <c r="R236" t="s" s="2">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="S236" t="s" s="2">
         <v>75</v>
@@ -29831,10 +29836,10 @@
     </row>
     <row r="237" hidden="true">
       <c r="A237" t="s" s="2">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B237" t="s" s="2">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C237" s="2"/>
       <c r="D237" t="s" s="2">
@@ -29929,7 +29934,7 @@
         <v>100</v>
       </c>
       <c r="AK237" t="s" s="2">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="AL237" t="s" s="2">
         <v>75</v>
@@ -29940,10 +29945,10 @@
     </row>
     <row r="238" hidden="true">
       <c r="A238" t="s" s="2">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B238" t="s" s="2">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C238" s="2"/>
       <c r="D238" t="s" s="2">
@@ -30049,14 +30054,14 @@
     </row>
     <row r="239" hidden="true">
       <c r="A239" t="s" s="2">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B239" t="s" s="2">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C239" s="2"/>
       <c r="D239" t="s" s="2">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="E239" s="2"/>
       <c r="F239" t="s" s="2">
@@ -30078,10 +30083,10 @@
         <v>103</v>
       </c>
       <c r="L239" t="s" s="2">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="M239" t="s" s="2">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="N239" t="s" s="2">
         <v>544</v>
@@ -30098,7 +30103,7 @@
         <v>75</v>
       </c>
       <c r="T239" t="s" s="2">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="U239" t="s" s="2">
         <v>75</v>
@@ -30134,7 +30139,7 @@
         <v>75</v>
       </c>
       <c r="AF239" t="s" s="2">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="AG239" t="s" s="2">
         <v>76</v>
@@ -30149,7 +30154,7 @@
         <v>100</v>
       </c>
       <c r="AK239" t="s" s="2">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="AL239" t="s" s="2">
         <v>75</v>
@@ -30160,14 +30165,14 @@
     </row>
     <row r="240" hidden="true">
       <c r="A240" t="s" s="2">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="B240" t="s" s="2">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="C240" s="2"/>
       <c r="D240" t="s" s="2">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="E240" s="2"/>
       <c r="F240" t="s" s="2">
@@ -30189,13 +30194,13 @@
         <v>103</v>
       </c>
       <c r="L240" t="s" s="2">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="M240" t="s" s="2">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="N240" t="s" s="2">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="O240" s="2"/>
       <c r="P240" t="s" s="2">
@@ -30209,7 +30214,7 @@
         <v>75</v>
       </c>
       <c r="T240" t="s" s="2">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="U240" t="s" s="2">
         <v>75</v>
@@ -30245,7 +30250,7 @@
         <v>75</v>
       </c>
       <c r="AF240" t="s" s="2">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="AG240" t="s" s="2">
         <v>76</v>
@@ -30271,14 +30276,14 @@
     </row>
     <row r="241" hidden="true">
       <c r="A241" t="s" s="2">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="B241" t="s" s="2">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="C241" s="2"/>
       <c r="D241" t="s" s="2">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="E241" s="2"/>
       <c r="F241" t="s" s="2">
@@ -30300,10 +30305,10 @@
         <v>103</v>
       </c>
       <c r="L241" t="s" s="2">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="M241" t="s" s="2">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="N241" t="s" s="2">
         <v>544</v>
@@ -30356,7 +30361,7 @@
         <v>75</v>
       </c>
       <c r="AF241" t="s" s="2">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="AG241" t="s" s="2">
         <v>76</v>
@@ -30382,14 +30387,14 @@
     </row>
     <row r="242" hidden="true">
       <c r="A242" t="s" s="2">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B242" t="s" s="2">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="C242" s="2"/>
       <c r="D242" t="s" s="2">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="E242" s="2"/>
       <c r="F242" t="s" s="2">
@@ -30411,10 +30416,10 @@
         <v>103</v>
       </c>
       <c r="L242" t="s" s="2">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="M242" t="s" s="2">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="N242" t="s" s="2">
         <v>544</v>
@@ -30431,7 +30436,7 @@
         <v>75</v>
       </c>
       <c r="T242" t="s" s="2">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="U242" t="s" s="2">
         <v>75</v>
@@ -30467,7 +30472,7 @@
         <v>75</v>
       </c>
       <c r="AF242" t="s" s="2">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="AG242" t="s" s="2">
         <v>76</v>
@@ -30482,7 +30487,7 @@
         <v>100</v>
       </c>
       <c r="AK242" t="s" s="2">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="AL242" t="s" s="2">
         <v>75</v>
@@ -30493,10 +30498,10 @@
     </row>
     <row r="243" hidden="true">
       <c r="A243" t="s" s="2">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="B243" t="s" s="2">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="C243" s="2"/>
       <c r="D243" t="s" s="2">
@@ -30522,13 +30527,13 @@
         <v>103</v>
       </c>
       <c r="L243" t="s" s="2">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="M243" t="s" s="2">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="N243" t="s" s="2">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="O243" s="2"/>
       <c r="P243" t="s" s="2">
@@ -30578,7 +30583,7 @@
         <v>75</v>
       </c>
       <c r="AF243" t="s" s="2">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="AG243" t="s" s="2">
         <v>76</v>
@@ -30604,10 +30609,10 @@
     </row>
     <row r="244" hidden="true">
       <c r="A244" t="s" s="2">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="B244" t="s" s="2">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C244" s="2"/>
       <c r="D244" t="s" s="2">
@@ -30633,16 +30638,16 @@
         <v>224</v>
       </c>
       <c r="L244" t="s" s="2">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="M244" t="s" s="2">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="N244" t="s" s="2">
         <v>387</v>
       </c>
       <c r="O244" t="s" s="2">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="P244" t="s" s="2">
         <v>75</v>
@@ -30655,7 +30660,7 @@
         <v>75</v>
       </c>
       <c r="T244" t="s" s="2">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="U244" t="s" s="2">
         <v>75</v>
@@ -30691,7 +30696,7 @@
         <v>75</v>
       </c>
       <c r="AF244" t="s" s="2">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="AG244" t="s" s="2">
         <v>76</v>
@@ -30717,10 +30722,10 @@
     </row>
     <row r="245" hidden="true">
       <c r="A245" t="s" s="2">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B245" t="s" s="2">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C245" s="2"/>
       <c r="D245" t="s" s="2">
@@ -30743,19 +30748,19 @@
         <v>87</v>
       </c>
       <c r="K245" t="s" s="2">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="L245" t="s" s="2">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="M245" t="s" s="2">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="N245" t="s" s="2">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="O245" t="s" s="2">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="P245" t="s" s="2">
         <v>75</v>
@@ -30804,7 +30809,7 @@
         <v>75</v>
       </c>
       <c r="AF245" t="s" s="2">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="AG245" t="s" s="2">
         <v>76</v>
@@ -30830,10 +30835,10 @@
     </row>
     <row r="246" hidden="true">
       <c r="A246" t="s" s="2">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B246" t="s" s="2">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="C246" s="2"/>
       <c r="D246" t="s" s="2">
@@ -30939,10 +30944,10 @@
     </row>
     <row r="247" hidden="true">
       <c r="A247" t="s" s="2">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B247" t="s" s="2">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="C247" s="2"/>
       <c r="D247" t="s" s="2">
@@ -31050,10 +31055,10 @@
     </row>
     <row r="248" hidden="true">
       <c r="A248" t="s" s="2">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B248" t="s" s="2">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="C248" s="2"/>
       <c r="D248" t="s" s="2">
@@ -31079,13 +31084,13 @@
         <v>103</v>
       </c>
       <c r="L248" t="s" s="2">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="M248" t="s" s="2">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="N248" t="s" s="2">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="O248" s="2"/>
       <c r="P248" t="s" s="2">
@@ -31135,7 +31140,7 @@
         <v>75</v>
       </c>
       <c r="AF248" t="s" s="2">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="AG248" t="s" s="2">
         <v>76</v>
@@ -31144,7 +31149,7 @@
         <v>86</v>
       </c>
       <c r="AI248" t="s" s="2">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="AJ248" t="s" s="2">
         <v>100</v>
@@ -31161,10 +31166,10 @@
     </row>
     <row r="249" hidden="true">
       <c r="A249" t="s" s="2">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B249" t="s" s="2">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C249" s="2"/>
       <c r="D249" t="s" s="2">
@@ -31190,13 +31195,13 @@
         <v>131</v>
       </c>
       <c r="L249" t="s" s="2">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="M249" t="s" s="2">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="N249" t="s" s="2">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="O249" s="2"/>
       <c r="P249" t="s" s="2">
@@ -31225,7 +31230,7 @@
         <v>147</v>
       </c>
       <c r="Y249" t="s" s="2">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="Z249" t="s" s="2">
         <v>510</v>
@@ -31246,7 +31251,7 @@
         <v>75</v>
       </c>
       <c r="AF249" t="s" s="2">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="AG249" t="s" s="2">
         <v>76</v>
@@ -31272,10 +31277,10 @@
     </row>
     <row r="250" hidden="true">
       <c r="A250" t="s" s="2">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B250" t="s" s="2">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C250" s="2"/>
       <c r="D250" t="s" s="2">
@@ -31301,13 +31306,13 @@
         <v>346</v>
       </c>
       <c r="L250" t="s" s="2">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="M250" t="s" s="2">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="N250" t="s" s="2">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="O250" s="2"/>
       <c r="P250" t="s" s="2">
@@ -31357,7 +31362,7 @@
         <v>75</v>
       </c>
       <c r="AF250" t="s" s="2">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="AG250" t="s" s="2">
         <v>76</v>
@@ -31383,10 +31388,10 @@
     </row>
     <row r="251" hidden="true">
       <c r="A251" t="s" s="2">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="B251" t="s" s="2">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="C251" s="2"/>
       <c r="D251" t="s" s="2">
@@ -31412,13 +31417,13 @@
         <v>103</v>
       </c>
       <c r="L251" t="s" s="2">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="M251" t="s" s="2">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="N251" t="s" s="2">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="O251" s="2"/>
       <c r="P251" t="s" s="2">
@@ -31468,7 +31473,7 @@
         <v>75</v>
       </c>
       <c r="AF251" t="s" s="2">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="AG251" t="s" s="2">
         <v>76</v>
@@ -31494,10 +31499,10 @@
     </row>
     <row r="252" hidden="true">
       <c r="A252" t="s" s="2">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B252" t="s" s="2">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="C252" s="2"/>
       <c r="D252" t="s" s="2">
@@ -31520,19 +31525,19 @@
         <v>75</v>
       </c>
       <c r="K252" t="s" s="2">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="L252" t="s" s="2">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="M252" t="s" s="2">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="N252" t="s" s="2">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="O252" t="s" s="2">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="P252" t="s" s="2">
         <v>75</v>
@@ -31581,7 +31586,7 @@
         <v>75</v>
       </c>
       <c r="AF252" t="s" s="2">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="AG252" t="s" s="2">
         <v>76</v>
@@ -31596,10 +31601,10 @@
         <v>100</v>
       </c>
       <c r="AK252" t="s" s="2">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="AL252" t="s" s="2">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="AM252" t="s" s="2">
         <v>75</v>
@@ -31607,10 +31612,10 @@
     </row>
     <row r="253" hidden="true">
       <c r="A253" t="s" s="2">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="B253" t="s" s="2">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" t="s" s="2">
@@ -31716,10 +31721,10 @@
     </row>
     <row r="254" hidden="true">
       <c r="A254" t="s" s="2">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B254" t="s" s="2">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" t="s" s="2">
@@ -31825,13 +31830,13 @@
     </row>
     <row r="255" hidden="true">
       <c r="A255" t="s" s="2">
+        <v>963</v>
+      </c>
+      <c r="B255" t="s" s="2">
         <v>962</v>
       </c>
-      <c r="B255" t="s" s="2">
-        <v>961</v>
-      </c>
       <c r="C255" t="s" s="2">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="D255" t="s" s="2">
         <v>75</v>
@@ -31853,13 +31858,13 @@
         <v>75</v>
       </c>
       <c r="K255" t="s" s="2">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="L255" t="s" s="2">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="M255" t="s" s="2">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="N255" s="2"/>
       <c r="O255" s="2"/>
@@ -31936,13 +31941,13 @@
     </row>
     <row r="256" hidden="true">
       <c r="A256" t="s" s="2">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B256" t="s" s="2">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="C256" t="s" s="2">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="D256" t="s" s="2">
         <v>75</v>
@@ -31964,13 +31969,13 @@
         <v>75</v>
       </c>
       <c r="K256" t="s" s="2">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="L256" t="s" s="2">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="M256" t="s" s="2">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="N256" s="2"/>
       <c r="O256" s="2"/>
@@ -32047,13 +32052,13 @@
     </row>
     <row r="257" hidden="true">
       <c r="A257" t="s" s="2">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B257" t="s" s="2">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="C257" t="s" s="2">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="D257" t="s" s="2">
         <v>75</v>
@@ -32075,13 +32080,13 @@
         <v>75</v>
       </c>
       <c r="K257" t="s" s="2">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="L257" t="s" s="2">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="M257" t="s" s="2">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="N257" s="2"/>
       <c r="O257" s="2"/>
@@ -32158,14 +32163,14 @@
     </row>
     <row r="258" hidden="true">
       <c r="A258" t="s" s="2">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="B258" t="s" s="2">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="C258" s="2"/>
       <c r="D258" t="s" s="2">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="E258" s="2"/>
       <c r="F258" t="s" s="2">
@@ -32187,10 +32192,10 @@
         <v>109</v>
       </c>
       <c r="L258" t="s" s="2">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="M258" t="s" s="2">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="N258" t="s" s="2">
         <v>112</v>
@@ -32245,7 +32250,7 @@
         <v>75</v>
       </c>
       <c r="AF258" t="s" s="2">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="AG258" t="s" s="2">
         <v>76</v>
@@ -32271,10 +32276,10 @@
     </row>
     <row r="259" hidden="true">
       <c r="A259" t="s" s="2">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="B259" t="s" s="2">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="C259" s="2"/>
       <c r="D259" t="s" s="2">
@@ -32300,16 +32305,16 @@
         <v>363</v>
       </c>
       <c r="L259" t="s" s="2">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="M259" t="s" s="2">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="N259" t="s" s="2">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="O259" t="s" s="2">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="P259" t="s" s="2">
         <v>75</v>
@@ -32338,7 +32343,7 @@
       </c>
       <c r="Y259" s="2"/>
       <c r="Z259" t="s" s="2">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="AA259" t="s" s="2">
         <v>75</v>
@@ -32356,7 +32361,7 @@
         <v>75</v>
       </c>
       <c r="AF259" t="s" s="2">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="AG259" t="s" s="2">
         <v>76</v>
@@ -32371,10 +32376,10 @@
         <v>100</v>
       </c>
       <c r="AK259" t="s" s="2">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="AL259" t="s" s="2">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="AM259" t="s" s="2">
         <v>75</v>
@@ -32382,10 +32387,10 @@
     </row>
     <row r="260" hidden="true">
       <c r="A260" t="s" s="2">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B260" t="s" s="2">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" t="s" s="2">
@@ -32408,19 +32413,19 @@
         <v>75</v>
       </c>
       <c r="K260" t="s" s="2">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="L260" t="s" s="2">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="M260" t="s" s="2">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="N260" t="s" s="2">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="O260" t="s" s="2">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="P260" t="s" s="2">
         <v>75</v>
@@ -32469,7 +32474,7 @@
         <v>75</v>
       </c>
       <c r="AF260" t="s" s="2">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="AG260" t="s" s="2">
         <v>76</v>
@@ -32484,10 +32489,10 @@
         <v>100</v>
       </c>
       <c r="AK260" t="s" s="2">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="AL260" t="s" s="2">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="AM260" t="s" s="2">
         <v>75</v>
@@ -32495,10 +32500,10 @@
     </row>
     <row r="261" hidden="true">
       <c r="A261" t="s" s="2">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B261" t="s" s="2">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" t="s" s="2">
@@ -32524,14 +32529,14 @@
         <v>653</v>
       </c>
       <c r="L261" t="s" s="2">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="M261" t="s" s="2">
         <v>655</v>
       </c>
       <c r="N261" s="2"/>
       <c r="O261" t="s" s="2">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="P261" t="s" s="2">
         <v>75</v>
@@ -32580,7 +32585,7 @@
         <v>75</v>
       </c>
       <c r="AF261" t="s" s="2">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="AG261" t="s" s="2">
         <v>76</v>
@@ -32592,13 +32597,13 @@
         <v>99</v>
       </c>
       <c r="AJ261" t="s" s="2">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="AK261" t="s" s="2">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="AL261" t="s" s="2">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="AM261" t="s" s="2">
         <v>75</v>
@@ -32606,10 +32611,10 @@
     </row>
     <row r="262" hidden="true">
       <c r="A262" t="s" s="2">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B262" t="s" s="2">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="C262" s="2"/>
       <c r="D262" t="s" s="2">
@@ -32715,10 +32720,10 @@
     </row>
     <row r="263" hidden="true">
       <c r="A263" t="s" s="2">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B263" t="s" s="2">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" t="s" s="2">
@@ -32824,10 +32829,10 @@
     </row>
     <row r="264" hidden="true">
       <c r="A264" t="s" s="2">
+        <v>1004</v>
+      </c>
+      <c r="B264" t="s" s="2">
         <v>1003</v>
-      </c>
-      <c r="B264" t="s" s="2">
-        <v>1002</v>
       </c>
       <c r="C264" t="s" s="2">
         <v>665</v>
@@ -32937,10 +32942,10 @@
     </row>
     <row r="265" hidden="true">
       <c r="A265" t="s" s="2">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B265" t="s" s="2">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C265" t="s" s="2">
         <v>679</v>
@@ -33048,10 +33053,10 @@
     </row>
     <row r="266" hidden="true">
       <c r="A266" t="s" s="2">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="B266" t="s" s="2">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C266" t="s" s="2">
         <v>674</v>
@@ -33159,10 +33164,10 @@
     </row>
     <row r="267" hidden="true">
       <c r="A267" t="s" s="2">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="B267" t="s" s="2">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C267" t="s" s="2">
         <v>669</v>
@@ -33190,7 +33195,7 @@
         <v>670</v>
       </c>
       <c r="L267" t="s" s="2">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="M267" t="s" s="2">
         <v>672</v>
@@ -33270,10 +33275,10 @@
     </row>
     <row r="268" hidden="true">
       <c r="A268" t="s" s="2">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B268" t="s" s="2">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C268" s="2"/>
       <c r="D268" t="s" s="2">
@@ -33381,10 +33386,10 @@
     </row>
     <row r="269" hidden="true">
       <c r="A269" t="s" s="2">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B269" t="s" s="2">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="C269" s="2"/>
       <c r="D269" t="s" s="2">
@@ -33494,10 +33499,10 @@
     </row>
     <row r="270" hidden="true">
       <c r="A270" t="s" s="2">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B270" t="s" s="2">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C270" s="2"/>
       <c r="D270" t="s" s="2">
@@ -33607,10 +33612,10 @@
     </row>
     <row r="271" hidden="true">
       <c r="A271" t="s" s="2">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B271" t="s" s="2">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="C271" s="2"/>
       <c r="D271" t="s" s="2">
@@ -33718,10 +33723,10 @@
     </row>
     <row r="272" hidden="true">
       <c r="A272" t="s" s="2">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="B272" t="s" s="2">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" t="s" s="2">
@@ -33829,10 +33834,10 @@
     </row>
     <row r="273" hidden="true">
       <c r="A273" t="s" s="2">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B273" t="s" s="2">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="C273" s="2"/>
       <c r="D273" t="s" s="2">
@@ -33858,7 +33863,7 @@
         <v>716</v>
       </c>
       <c r="L273" t="s" s="2">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="M273" t="s" s="2">
         <v>718</v>
@@ -33867,7 +33872,7 @@
         <v>719</v>
       </c>
       <c r="O273" t="s" s="2">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="P273" t="s" s="2">
         <v>75</v>
@@ -33916,7 +33921,7 @@
         <v>75</v>
       </c>
       <c r="AF273" t="s" s="2">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="AG273" t="s" s="2">
         <v>76</v>
@@ -33942,10 +33947,10 @@
     </row>
     <row r="274" hidden="true">
       <c r="A274" t="s" s="2">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B274" t="s" s="2">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C274" s="2"/>
       <c r="D274" t="s" s="2">
@@ -33968,19 +33973,19 @@
         <v>75</v>
       </c>
       <c r="K274" t="s" s="2">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="L274" t="s" s="2">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="M274" t="s" s="2">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="N274" t="s" s="2">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="O274" t="s" s="2">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="P274" t="s" s="2">
         <v>75</v>
@@ -34029,7 +34034,7 @@
         <v>75</v>
       </c>
       <c r="AF274" t="s" s="2">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="AG274" t="s" s="2">
         <v>76</v>

</xml_diff>